<commit_message>
Fix Sample and Subject enum tests
</commit_message>
<xml_diff>
--- a/InputFiles/API/Federation/AllowedValues.xlsx
+++ b/InputFiles/API/Federation/AllowedValues.xlsx
@@ -8,12 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/API/Federation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5376AA9A-D250-794C-832E-D79531EFAD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16582E2D-0D6A-074D-9A1A-FB2A85B0B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{8F72063A-9150-2546-A2F6-5AE255D363FD}"/>
+    <workbookView xWindow="2080" yWindow="-26920" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{8F72063A-9150-2546-A2F6-5AE255D363FD}"/>
   </bookViews>
   <sheets>
     <sheet name="FileType" sheetId="2" r:id="rId1"/>
+    <sheet name="SubjEthn" sheetId="3" r:id="rId2"/>
+    <sheet name="SubjSex" sheetId="4" r:id="rId3"/>
+    <sheet name="SubjRace" sheetId="5" r:id="rId4"/>
+    <sheet name="SubjVital" sheetId="6" r:id="rId5"/>
+    <sheet name="SampDisPh" sheetId="7" r:id="rId6"/>
+    <sheet name="SampLibSel" sheetId="8" r:id="rId7"/>
+    <sheet name="SampLibStr" sheetId="9" r:id="rId8"/>
+    <sheet name="SampLibSrc" sheetId="10" r:id="rId9"/>
+    <sheet name="SampPresrv" sheetId="11" r:id="rId10"/>
+    <sheet name="SampSpeci" sheetId="12" r:id="rId11"/>
+    <sheet name="SampTiss" sheetId="13" r:id="rId12"/>
+    <sheet name="SampTumor" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="179">
   <si>
     <t>ADF</t>
   </si>
@@ -276,6 +288,303 @@
   </si>
   <si>
     <t>ZIP</t>
+  </si>
+  <si>
+    <t>Not allowed to collect</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Not Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Not reported</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>UNDIFFERENTIATED</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or other Pacific Islander</t>
+  </si>
+  <si>
+    <t>Not Reported</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Alive</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Unspecified</t>
+  </si>
+  <si>
+    <t>Post-Mortem</t>
+  </si>
+  <si>
+    <t>Initial Diagnosis</t>
+  </si>
+  <si>
+    <t>Progression</t>
+  </si>
+  <si>
+    <t>Refractory</t>
+  </si>
+  <si>
+    <t>Relapse</t>
+  </si>
+  <si>
+    <t>Relapse/Progression</t>
+  </si>
+  <si>
+    <t>Random PCR</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Hybrid Selection</t>
+  </si>
+  <si>
+    <t>rRNA Depletion</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Poly-A Enriched Genomic Library</t>
+  </si>
+  <si>
+    <t>AMPLICON</t>
+  </si>
+  <si>
+    <t>ATAC-Seq</t>
+  </si>
+  <si>
+    <t>Bisulfite-Seq</t>
+  </si>
+  <si>
+    <t>ChIA-PET</t>
+  </si>
+  <si>
+    <t>ChIP-Seq</t>
+  </si>
+  <si>
+    <t>CLONE</t>
+  </si>
+  <si>
+    <t>CLONEEND</t>
+  </si>
+  <si>
+    <t>CTS</t>
+  </si>
+  <si>
+    <t>DNA-Seq</t>
+  </si>
+  <si>
+    <t>DNase-Hypersensitivity</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>FAIRE-seq</t>
+  </si>
+  <si>
+    <t>FINISHING</t>
+  </si>
+  <si>
+    <t>FL-cDNA</t>
+  </si>
+  <si>
+    <t>Hi-C</t>
+  </si>
+  <si>
+    <t>MBD-Seq</t>
+  </si>
+  <si>
+    <t>MeDIP-Seq</t>
+  </si>
+  <si>
+    <t>miRNA-Seq</t>
+  </si>
+  <si>
+    <t>MNase-Seq</t>
+  </si>
+  <si>
+    <t>MRE-Seq</t>
+  </si>
+  <si>
+    <t>ncRNA-Seq</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>POOLCLONE</t>
+  </si>
+  <si>
+    <t>RAD-Seq</t>
+  </si>
+  <si>
+    <t>RIP-Seq</t>
+  </si>
+  <si>
+    <t>RNA-Seq</t>
+  </si>
+  <si>
+    <t>SELEX</t>
+  </si>
+  <si>
+    <t>snATAC-Seq</t>
+  </si>
+  <si>
+    <t>ssRNA-seq</t>
+  </si>
+  <si>
+    <t>Synthetic-Long-Read</t>
+  </si>
+  <si>
+    <t>Targeted-Capture</t>
+  </si>
+  <si>
+    <t>Tethered Chromatin Conformation Capture</t>
+  </si>
+  <si>
+    <t>Tn-Seq</t>
+  </si>
+  <si>
+    <t>WCS</t>
+  </si>
+  <si>
+    <t>WGA</t>
+  </si>
+  <si>
+    <t>WGS</t>
+  </si>
+  <si>
+    <t>WXS</t>
+  </si>
+  <si>
+    <t>Bulk Cells</t>
+  </si>
+  <si>
+    <t>Bulk Nuclei</t>
+  </si>
+  <si>
+    <t>Bulk Tissue</t>
+  </si>
+  <si>
+    <t>Single-cells</t>
+  </si>
+  <si>
+    <t>Single-nuclei</t>
+  </si>
+  <si>
+    <t>-80 degrees C</t>
+  </si>
+  <si>
+    <t>Cryopreserved</t>
+  </si>
+  <si>
+    <t>EDTA</t>
+  </si>
+  <si>
+    <t>FFPE</t>
+  </si>
+  <si>
+    <t>Formalin Fixed - Buffered</t>
+  </si>
+  <si>
+    <t>Formalin Fixed - Unbuffered</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>Fresh Dissociated</t>
+  </si>
+  <si>
+    <t>Fresh Dissociated and Single Cell Sorted</t>
+  </si>
+  <si>
+    <t>Fresh Dissociated and Single Cell Sorted into Plates</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>Liquid Nitrogen</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>Snap Frozen</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>RNA</t>
+  </si>
+  <si>
+    <t>Abnormal</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Peritumoral</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>Non-neoplastic</t>
+  </si>
+  <si>
+    <t>Unavailable</t>
+  </si>
+  <si>
+    <t>Metastatic</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Regional</t>
   </si>
 </sst>
 </file>
@@ -649,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDC7E7D-67B1-E74F-95AA-67A4A1736614}">
   <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
@@ -1061,4 +1370,787 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CBA0B7-C2FD-F546-80E0-024FAA266547}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F19E49D-E750-474D-B49A-7F44CBB3D31F}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2260463-E625-2642-AA75-995111FA6039}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E096A7-B0F5-4B4D-B6DB-BC0672186A4D}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1D6B96-7285-604A-81E3-2DB1C7B968A4}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC82661-6CE5-194D-9C87-A842CDDF8C0E}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FBB89E-B037-0245-B99F-FE3917D1A32B}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A883415-8D72-5645-9578-A9F7D31A654C}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B976C21-91B9-7F47-8FA1-4D2E795C1211}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA616C0-3A47-5F4F-B539-988E7D0961D6}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A542D5-DA0D-E74C-BC72-EC61A7242CDA}">
+  <dimension ref="A1:A37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BEA9D7-307D-0749-90C8-581D280D88DA}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Federation test case additions
</commit_message>
<xml_diff>
--- a/InputFiles/API/Federation/AllowedValues.xlsx
+++ b/InputFiles/API/Federation/AllowedValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/API/Federation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/API/Federation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16582E2D-0D6A-074D-9A1A-FB2A85B0B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88207591-BE1A-B746-B2CB-B08F6F3DFB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="-26920" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{8F72063A-9150-2546-A2F6-5AE255D363FD}"/>
+    <workbookView xWindow="19140" yWindow="-25920" windowWidth="28040" windowHeight="17440" firstSheet="1" activeTab="13" xr2:uid="{8F72063A-9150-2546-A2F6-5AE255D363FD}"/>
   </bookViews>
   <sheets>
     <sheet name="FileType" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="SampSpeci" sheetId="12" r:id="rId11"/>
     <sheet name="SampTiss" sheetId="13" r:id="rId12"/>
     <sheet name="SampTumor" sheetId="14" r:id="rId13"/>
+    <sheet name="SampTumGrd" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
   <si>
     <t>ADF</t>
   </si>
@@ -560,9 +561,6 @@
     <t>RNA</t>
   </si>
   <si>
-    <t>Abnormal</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -572,12 +570,6 @@
     <t>Tumor</t>
   </si>
   <si>
-    <t>Non-neoplastic</t>
-  </si>
-  <si>
-    <t>Unavailable</t>
-  </si>
-  <si>
     <t>Metastatic</t>
   </si>
   <si>
@@ -585,6 +577,27 @@
   </si>
   <si>
     <t>Regional</t>
+  </si>
+  <si>
+    <t>G1 Low Grade</t>
+  </si>
+  <si>
+    <t>G2 Intermediate Grade</t>
+  </si>
+  <si>
+    <t>G3 High Grade</t>
+  </si>
+  <si>
+    <t>G4 Anaplastic</t>
+  </si>
+  <si>
+    <t>GB Borderline</t>
+  </si>
+  <si>
+    <t>GX Grade Cannot Be Assessed</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -1502,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2260463-E625-2642-AA75-995111FA6039}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,27 +1548,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1578,7 +1571,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -1588,16 +1581,79 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EB17FA-99E4-E04E-8B4B-4BE4328D4350}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1691,7 +1747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FBB89E-B037-0245-B99F-FE3917D1A32B}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>